<commit_message>
dodal lineup editor; em rest je down :(((
</commit_message>
<xml_diff>
--- a/bands_corrected_extended.xlsx
+++ b/bands_corrected_extended.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleptes\Documents\programming\Python\metaldays_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3B88A3D7-3CDE-4FA3-B87C-506484AE1A77}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{381D7E42-7262-4973-9EFC-93EE5EE71A59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="388">
   <si>
     <t>Band</t>
   </si>
@@ -1124,6 +1124,66 @@
   </si>
   <si>
     <t>Atmospheric Black/Doom Metal/Ambient</t>
+  </si>
+  <si>
+    <t>LEPROUS</t>
+  </si>
+  <si>
+    <t>ALESTORM</t>
+  </si>
+  <si>
+    <t>ELUVEITIE</t>
+  </si>
+  <si>
+    <t>BEHEMOTH</t>
+  </si>
+  <si>
+    <t>CORONER</t>
+  </si>
+  <si>
+    <t>ENSIFERUM</t>
+  </si>
+  <si>
+    <t>ACCEPT</t>
+  </si>
+  <si>
+    <t>WATAIN</t>
+  </si>
+  <si>
+    <t>LOUDNESS</t>
+  </si>
+  <si>
+    <t>IGORRR</t>
+  </si>
+  <si>
+    <t>KATAKLYSM</t>
+  </si>
+  <si>
+    <t>M2TM</t>
+  </si>
+  <si>
+    <t>OBITUARY</t>
+  </si>
+  <si>
+    <t>BLACK STAR RIDERS</t>
+  </si>
+  <si>
+    <t>HATEBREED</t>
+  </si>
+  <si>
+    <t>JUDAS PRIEST</t>
+  </si>
+  <si>
+    <t>MUNICIPAL WASTE</t>
+  </si>
+  <si>
+    <t>CANNIBAL CORPSE</t>
+  </si>
+  <si>
+    <t>EPICA</t>
+  </si>
+  <si>
+    <t>CHILDREN OF BODOM</t>
   </si>
 </sst>
 </file>
@@ -1964,10 +2024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4211,6 +4271,106 @@
         <v>340</v>
       </c>
     </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>387</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:F117">
     <sortCondition descending="1" ref="E2"/>

</xml_diff>